<commit_message>
added the origin file, and updated the results
</commit_message>
<xml_diff>
--- a/IEEETransactionOnIntelligent/scenarios (version 1).xlsb.xlsx
+++ b/IEEETransactionOnIntelligent/scenarios (version 1).xlsb.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\matlab_workspace\SchedulingSimulation\IEEETransactionOnIntelligent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CAEDB5-A404-45C0-98B4-25AB64C4836D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20A8D33-7522-4D98-839B-A5BA00A1E414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43425" yWindow="3645" windowWidth="15300" windowHeight="7815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TrafficMetric" sheetId="1" r:id="rId1"/>
     <sheet name="different Seeds" sheetId="2" r:id="rId2"/>
-    <sheet name="Histogram" sheetId="3" r:id="rId3"/>
+    <sheet name="Scenario1-revised" sheetId="5" r:id="rId3"/>
     <sheet name="Scenario2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="37">
   <si>
     <t>u_min</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t xml:space="preserve">Done </t>
+  </si>
+  <si>
+    <t xml:space="preserve">histogram </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph </t>
+  </si>
+  <si>
+    <t>Seed 42</t>
+  </si>
+  <si>
+    <t>Seed42</t>
   </si>
 </sst>
 </file>
@@ -892,7 +904,7 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K10"/>
+      <selection activeCell="N14" sqref="A14:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB574D0-D7A2-47DE-BC32-9F6E57DEC63E}">
   <dimension ref="A3:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3091,15 +3103,1458 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189455D5-5090-490B-AA3B-AB29451C298A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9648945-6AF8-4AFE-93CD-85E1ADD724BE}">
+  <dimension ref="A3:R41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="15"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D3" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="69"/>
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>42</v>
+      </c>
+      <c r="B6" s="19">
+        <v>6</v>
+      </c>
+      <c r="C6" s="20">
+        <v>400</v>
+      </c>
+      <c r="D6" s="19">
+        <v>41.47</v>
+      </c>
+      <c r="E6" s="20">
+        <v>58.06</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="21">
+        <f t="shared" ref="G6:G30" si="0">-(D6-E6)/E6</f>
+        <v>0.28573889080261805</v>
+      </c>
+      <c r="H6" s="19">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="I6" s="19">
+        <v>12.69</v>
+      </c>
+      <c r="J6" s="19">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="K6" s="19">
+        <v>1.35</v>
+      </c>
+      <c r="L6" s="19">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="M6" s="19">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="N6" s="19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>42</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20">
+        <v>600</v>
+      </c>
+      <c r="D7" s="19">
+        <v>44.33</v>
+      </c>
+      <c r="E7" s="22">
+        <v>60.48</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="21">
+        <f t="shared" si="0"/>
+        <v>0.26703042328042326</v>
+      </c>
+      <c r="H7" s="19">
+        <v>16.78</v>
+      </c>
+      <c r="I7" s="19">
+        <v>12.3</v>
+      </c>
+      <c r="J7" s="19">
+        <v>1.78</v>
+      </c>
+      <c r="K7" s="19">
+        <v>1.38</v>
+      </c>
+      <c r="L7" s="19">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="M7" s="19">
+        <v>7.9336599999999993E-2</v>
+      </c>
+      <c r="N7" s="19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>42</v>
+      </c>
+      <c r="B8" s="19">
+        <v>4</v>
+      </c>
+      <c r="C8" s="20">
+        <v>800</v>
+      </c>
+      <c r="D8" s="19">
+        <v>43.97</v>
+      </c>
+      <c r="E8" s="20">
+        <v>65.680000000000007</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="21">
+        <f t="shared" si="0"/>
+        <v>0.3305420219244824</v>
+      </c>
+      <c r="H8" s="19">
+        <v>17.09</v>
+      </c>
+      <c r="I8" s="19">
+        <v>11.54</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1.82</v>
+      </c>
+      <c r="K8" s="19">
+        <v>1.34</v>
+      </c>
+      <c r="L8" s="19">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="M8" s="19">
+        <v>8.0891699999999997E-2</v>
+      </c>
+      <c r="N8" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>42</v>
+      </c>
+      <c r="B9" s="19">
+        <v>7</v>
+      </c>
+      <c r="C9" s="20">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="19">
+        <v>46.71</v>
+      </c>
+      <c r="E9" s="20">
+        <v>70.38</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="21">
+        <f t="shared" si="0"/>
+        <v>0.33631713554987208</v>
+      </c>
+      <c r="H9" s="19">
+        <v>16.09</v>
+      </c>
+      <c r="I9" s="19">
+        <v>11.02</v>
+      </c>
+      <c r="J9" s="19">
+        <v>1.64</v>
+      </c>
+      <c r="K9" s="19">
+        <v>1.29</v>
+      </c>
+      <c r="L9" s="19">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="M9" s="19">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="N9" s="19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>42</v>
+      </c>
+      <c r="B10" s="19">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20">
+        <v>1200</v>
+      </c>
+      <c r="D10" s="19">
+        <v>48.42</v>
+      </c>
+      <c r="E10" s="20">
+        <v>73.66</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="21">
+        <f t="shared" si="0"/>
+        <v>0.34265544393157749</v>
+      </c>
+      <c r="H10" s="19">
+        <v>15.57</v>
+      </c>
+      <c r="I10" s="19">
+        <v>10.68</v>
+      </c>
+      <c r="J10" s="19">
+        <v>1.59</v>
+      </c>
+      <c r="K10" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="L10" s="19">
+        <v>7.5899999999999995E-2</v>
+      </c>
+      <c r="M10" s="19">
+        <v>8.1159200000000001E-2</v>
+      </c>
+      <c r="N10" s="19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11" s="13">
+        <v>6</v>
+      </c>
+      <c r="C11" s="14">
+        <v>400</v>
+      </c>
+      <c r="D11" s="13">
+        <v>39.74</v>
+      </c>
+      <c r="E11" s="14">
+        <v>52.23</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="18">
+        <f t="shared" si="0"/>
+        <v>0.23913459697491854</v>
+      </c>
+      <c r="H11" s="14">
+        <v>18</v>
+      </c>
+      <c r="I11" s="13">
+        <v>14.04</v>
+      </c>
+      <c r="J11" s="14">
+        <v>1.97</v>
+      </c>
+      <c r="K11" s="13">
+        <v>1.57</v>
+      </c>
+      <c r="L11" s="14">
+        <v>7.8502299999999997E-2</v>
+      </c>
+      <c r="M11" s="13">
+        <v>7.80608E-2</v>
+      </c>
+      <c r="N11" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14">
+        <v>600</v>
+      </c>
+      <c r="D12" s="13">
+        <v>41.96</v>
+      </c>
+      <c r="E12" s="14">
+        <v>57.18</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="18">
+        <f t="shared" si="0"/>
+        <v>0.26617698495977615</v>
+      </c>
+      <c r="H12" s="14">
+        <v>17.39</v>
+      </c>
+      <c r="I12" s="13">
+        <v>13.36</v>
+      </c>
+      <c r="J12" s="14">
+        <v>1.73</v>
+      </c>
+      <c r="K12" s="13">
+        <v>1.55</v>
+      </c>
+      <c r="L12" s="14">
+        <v>7.22719E-2</v>
+      </c>
+      <c r="M12" s="13">
+        <v>8.0457799999999996E-2</v>
+      </c>
+      <c r="N12" s="13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" s="13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14">
+        <v>800</v>
+      </c>
+      <c r="D13" s="13">
+        <v>44.41</v>
+      </c>
+      <c r="E13" s="14">
+        <v>65.150000000000006</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="18">
+        <f t="shared" si="0"/>
+        <v>0.31834228702993106</v>
+      </c>
+      <c r="H13" s="14">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="I13" s="13">
+        <v>11.73</v>
+      </c>
+      <c r="J13" s="14">
+        <v>1.74</v>
+      </c>
+      <c r="K13" s="13">
+        <v>1.38</v>
+      </c>
+      <c r="L13" s="14">
+        <v>7.6975000000000002E-2</v>
+      </c>
+      <c r="M13" s="13">
+        <v>8.0603099999999997E-2</v>
+      </c>
+      <c r="N13" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" s="13">
+        <v>7</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="13">
+        <v>47.15</v>
+      </c>
+      <c r="E14" s="14">
+        <v>72.92</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="18">
+        <f t="shared" si="0"/>
+        <v>0.35340098738343395</v>
+      </c>
+      <c r="H14" s="14">
+        <v>15.9</v>
+      </c>
+      <c r="I14" s="13">
+        <v>10.98</v>
+      </c>
+      <c r="J14" s="14">
+        <v>1.6</v>
+      </c>
+      <c r="K14" s="13">
+        <v>1.26</v>
+      </c>
+      <c r="L14" s="14">
+        <v>7.5179399999999993E-2</v>
+      </c>
+      <c r="M14" s="13">
+        <v>7.8747899999999996E-2</v>
+      </c>
+      <c r="N14" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="13">
+        <v>8</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1200</v>
+      </c>
+      <c r="D15" s="13">
+        <v>48.59</v>
+      </c>
+      <c r="E15" s="14">
+        <v>78.09</v>
+      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="18">
+        <f t="shared" si="0"/>
+        <v>0.37776924061979766</v>
+      </c>
+      <c r="H15" s="14">
+        <v>15.25</v>
+      </c>
+      <c r="I15" s="13">
+        <v>11.3</v>
+      </c>
+      <c r="J15" s="14">
+        <v>1.54</v>
+      </c>
+      <c r="K15" s="13">
+        <v>1.17</v>
+      </c>
+      <c r="L15" s="14">
+        <v>7.4560500000000002E-2</v>
+      </c>
+      <c r="M15" s="13">
+        <v>7.3347999999999997E-2</v>
+      </c>
+      <c r="N15" s="13">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="19">
+        <v>6</v>
+      </c>
+      <c r="C16" s="20">
+        <v>400</v>
+      </c>
+      <c r="D16" s="19">
+        <v>41.02</v>
+      </c>
+      <c r="E16" s="20">
+        <v>42.45</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="21">
+        <f t="shared" si="0"/>
+        <v>3.3686690223792691E-2</v>
+      </c>
+      <c r="H16" s="19">
+        <v>17.84</v>
+      </c>
+      <c r="I16" s="19">
+        <v>16.739999999999998</v>
+      </c>
+      <c r="J16" s="19">
+        <v>1.99</v>
+      </c>
+      <c r="K16" s="19">
+        <v>1.68</v>
+      </c>
+      <c r="L16" s="19">
+        <v>8.1463499999999994E-2</v>
+      </c>
+      <c r="M16" s="19">
+        <v>6.9698099999999999E-2</v>
+      </c>
+      <c r="N16" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="19">
+        <v>1</v>
+      </c>
+      <c r="C17" s="20">
+        <v>600</v>
+      </c>
+      <c r="D17" s="19">
+        <v>40.619999999999997</v>
+      </c>
+      <c r="E17" s="22">
+        <v>54.72</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="21">
+        <f t="shared" si="0"/>
+        <v>0.25767543859649128</v>
+      </c>
+      <c r="H17" s="19">
+        <v>18.05</v>
+      </c>
+      <c r="I17" s="19">
+        <v>13.23</v>
+      </c>
+      <c r="J17" s="19">
+        <v>2.08</v>
+      </c>
+      <c r="K17" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="L17" s="19">
+        <v>8.3872600000000005E-2</v>
+      </c>
+      <c r="M17" s="19">
+        <v>7.9600000000000004E-2</v>
+      </c>
+      <c r="N17" s="19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="19">
+        <v>4</v>
+      </c>
+      <c r="C18" s="20">
+        <v>800</v>
+      </c>
+      <c r="D18" s="19">
+        <v>41.81</v>
+      </c>
+      <c r="E18" s="20">
+        <v>58.5</v>
+      </c>
+      <c r="F18" s="27"/>
+      <c r="G18" s="21">
+        <f t="shared" si="0"/>
+        <v>0.28529914529914524</v>
+      </c>
+      <c r="H18" s="19">
+        <v>17.64</v>
+      </c>
+      <c r="I18" s="19">
+        <v>12.39</v>
+      </c>
+      <c r="J18" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="K18" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="L18" s="19">
+        <v>7.8952599999999998E-2</v>
+      </c>
+      <c r="M18" s="19">
+        <v>7.8953800000000005E-2</v>
+      </c>
+      <c r="N18" s="19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" s="19">
+        <v>7</v>
+      </c>
+      <c r="C19" s="20">
+        <v>1000</v>
+      </c>
+      <c r="D19" s="19">
+        <v>44.86</v>
+      </c>
+      <c r="E19" s="20">
+        <v>62.53</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="21">
+        <f t="shared" si="0"/>
+        <v>0.28258435950743643</v>
+      </c>
+      <c r="H19" s="19">
+        <v>16.53</v>
+      </c>
+      <c r="I19" s="19">
+        <v>11.81</v>
+      </c>
+      <c r="J19" s="19">
+        <v>1.73</v>
+      </c>
+      <c r="K19" s="19">
+        <v>1.38</v>
+      </c>
+      <c r="L19" s="19">
+        <v>7.6486799999999994E-2</v>
+      </c>
+      <c r="M19" s="19">
+        <v>8.0742400000000006E-2</v>
+      </c>
+      <c r="N19" s="19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" s="19">
+        <v>8</v>
+      </c>
+      <c r="C20" s="20">
+        <v>1200</v>
+      </c>
+      <c r="D20" s="19">
+        <v>45.13</v>
+      </c>
+      <c r="E20" s="20">
+        <v>64.19</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="21">
+        <f t="shared" si="0"/>
+        <v>0.29693098613491192</v>
+      </c>
+      <c r="H20" s="19">
+        <v>16.420000000000002</v>
+      </c>
+      <c r="I20" s="19">
+        <v>11.56</v>
+      </c>
+      <c r="J20" s="19">
+        <v>1.66</v>
+      </c>
+      <c r="K20" s="19">
+        <v>1.33</v>
+      </c>
+      <c r="L20" s="19">
+        <v>7.3701100000000005E-2</v>
+      </c>
+      <c r="M20" s="19">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="N20" s="19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" s="13">
+        <v>6</v>
+      </c>
+      <c r="C21" s="14">
+        <v>400</v>
+      </c>
+      <c r="D21" s="13">
+        <v>41.56</v>
+      </c>
+      <c r="E21" s="14">
+        <v>56.24</v>
+      </c>
+      <c r="F21" s="27"/>
+      <c r="G21" s="18">
+        <f t="shared" si="0"/>
+        <v>0.26102418207681366</v>
+      </c>
+      <c r="H21" s="14">
+        <v>17.79</v>
+      </c>
+      <c r="I21" s="13">
+        <v>12.91</v>
+      </c>
+      <c r="J21" s="14">
+        <v>2</v>
+      </c>
+      <c r="K21" s="13">
+        <v>1.48</v>
+      </c>
+      <c r="L21" s="14">
+        <v>8.3537299999999995E-2</v>
+      </c>
+      <c r="M21" s="13">
+        <v>8.1308699999999998E-2</v>
+      </c>
+      <c r="N21" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1</v>
+      </c>
+      <c r="C22" s="14">
+        <v>600</v>
+      </c>
+      <c r="D22" s="13">
+        <v>41.04</v>
+      </c>
+      <c r="E22" s="14">
+        <v>58.04</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="18">
+        <f t="shared" si="0"/>
+        <v>0.29290144727773948</v>
+      </c>
+      <c r="H22" s="14">
+        <v>17.88</v>
+      </c>
+      <c r="I22" s="13">
+        <v>12.56</v>
+      </c>
+      <c r="J22" s="14">
+        <v>2</v>
+      </c>
+      <c r="K22" s="13">
+        <v>1.4</v>
+      </c>
+      <c r="L22" s="14">
+        <v>8.2019300000000003E-2</v>
+      </c>
+      <c r="M22" s="13">
+        <v>7.7943200000000004E-2</v>
+      </c>
+      <c r="N22" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="13">
+        <v>4</v>
+      </c>
+      <c r="C23" s="14">
+        <v>800</v>
+      </c>
+      <c r="D23" s="13">
+        <v>42.18</v>
+      </c>
+      <c r="E23" s="14">
+        <v>61.15</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="18">
+        <f t="shared" si="0"/>
+        <v>0.31022076860179887</v>
+      </c>
+      <c r="H23" s="14">
+        <v>17.11</v>
+      </c>
+      <c r="I23" s="13">
+        <v>12.57</v>
+      </c>
+      <c r="J23" s="14">
+        <v>1.82</v>
+      </c>
+      <c r="K23" s="13">
+        <v>1.35</v>
+      </c>
+      <c r="L23" s="14">
+        <v>7.6481499999999994E-2</v>
+      </c>
+      <c r="M23" s="13">
+        <v>7.6056399999999996E-2</v>
+      </c>
+      <c r="N23" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" s="13">
+        <v>7</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D24" s="13">
+        <v>46.62</v>
+      </c>
+      <c r="E24" s="14">
+        <v>68.86</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="18">
+        <f t="shared" si="0"/>
+        <v>0.32297415045018885</v>
+      </c>
+      <c r="H24" s="14">
+        <v>15.81</v>
+      </c>
+      <c r="I24" s="13">
+        <v>11.77</v>
+      </c>
+      <c r="J24" s="14">
+        <v>1.56</v>
+      </c>
+      <c r="K24" s="13">
+        <v>1.28</v>
+      </c>
+      <c r="L24" s="14">
+        <v>7.1913400000000002E-2</v>
+      </c>
+      <c r="M24" s="13">
+        <v>7.6330499999999996E-2</v>
+      </c>
+      <c r="N24" s="13">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" s="13">
+        <v>8</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1200</v>
+      </c>
+      <c r="D25" s="13">
+        <v>49.69</v>
+      </c>
+      <c r="E25" s="14">
+        <v>68.349999999999994</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="18">
+        <f t="shared" si="0"/>
+        <v>0.27300658376005849</v>
+      </c>
+      <c r="H25" s="14">
+        <v>14.88</v>
+      </c>
+      <c r="I25" s="13">
+        <v>12</v>
+      </c>
+      <c r="J25" s="14">
+        <v>1.51</v>
+      </c>
+      <c r="K25" s="13">
+        <v>1.32</v>
+      </c>
+      <c r="L25" s="14">
+        <v>7.4201900000000001E-2</v>
+      </c>
+      <c r="M25" s="13">
+        <v>7.5161599999999995E-2</v>
+      </c>
+      <c r="N25" s="13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="19">
+        <v>6</v>
+      </c>
+      <c r="C26" s="20">
+        <v>400</v>
+      </c>
+      <c r="D26" s="19">
+        <v>40.26</v>
+      </c>
+      <c r="E26" s="20">
+        <v>50.47</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="21">
+        <f t="shared" si="0"/>
+        <v>0.20229839508618983</v>
+      </c>
+      <c r="H26" s="19">
+        <v>18.03</v>
+      </c>
+      <c r="I26" s="19">
+        <v>20.23</v>
+      </c>
+      <c r="J26" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="K26" s="19">
+        <v>1.56</v>
+      </c>
+      <c r="L26" s="19">
+        <v>8.4126900000000004E-2</v>
+      </c>
+      <c r="M26" s="19">
+        <v>7.6060000000000003E-2</v>
+      </c>
+      <c r="N26" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="19">
+        <v>1</v>
+      </c>
+      <c r="C27" s="20">
+        <v>600</v>
+      </c>
+      <c r="D27" s="19">
+        <v>41.33</v>
+      </c>
+      <c r="E27" s="22">
+        <v>57.16</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="21">
+        <f t="shared" si="0"/>
+        <v>0.27694191742477253</v>
+      </c>
+      <c r="H27" s="19">
+        <v>17.87</v>
+      </c>
+      <c r="I27" s="19">
+        <v>12.53</v>
+      </c>
+      <c r="J27" s="19">
+        <v>2.02</v>
+      </c>
+      <c r="K27" s="19">
+        <v>1.42</v>
+      </c>
+      <c r="L27" s="19">
+        <v>8.2577330000000004E-2</v>
+      </c>
+      <c r="M27" s="19">
+        <v>7.8288999999999997E-2</v>
+      </c>
+      <c r="N27" s="19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="19">
+        <v>4</v>
+      </c>
+      <c r="C28" s="20">
+        <v>800</v>
+      </c>
+      <c r="D28" s="19">
+        <v>43.95</v>
+      </c>
+      <c r="E28" s="20">
+        <v>66.02</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="21">
+        <f t="shared" si="0"/>
+        <v>0.33429263859436525</v>
+      </c>
+      <c r="H28" s="19">
+        <v>16.75</v>
+      </c>
+      <c r="I28" s="19">
+        <v>11.66</v>
+      </c>
+      <c r="J28" s="19">
+        <v>1.71</v>
+      </c>
+      <c r="K28" s="19">
+        <v>1.27</v>
+      </c>
+      <c r="L28" s="19">
+        <v>7.3809100000000002E-2</v>
+      </c>
+      <c r="M28" s="19">
+        <v>7.7808000000000002E-2</v>
+      </c>
+      <c r="N28" s="19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="19">
+        <v>7</v>
+      </c>
+      <c r="C29" s="20">
+        <v>1000</v>
+      </c>
+      <c r="D29" s="19">
+        <v>47.59</v>
+      </c>
+      <c r="E29" s="20">
+        <v>69.430000000000007</v>
+      </c>
+      <c r="F29" s="27"/>
+      <c r="G29" s="21">
+        <f t="shared" si="0"/>
+        <v>0.31456142877718568</v>
+      </c>
+      <c r="H29" s="19">
+        <v>15.58</v>
+      </c>
+      <c r="I29" s="19">
+        <v>11.41</v>
+      </c>
+      <c r="J29" s="19">
+        <v>1.56</v>
+      </c>
+      <c r="K29" s="19">
+        <v>1.24</v>
+      </c>
+      <c r="L29" s="19">
+        <v>7.2888679999999997E-2</v>
+      </c>
+      <c r="M29" s="19">
+        <v>7.6015200000000005E-2</v>
+      </c>
+      <c r="N29" s="19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" s="19">
+        <v>8</v>
+      </c>
+      <c r="C30" s="20">
+        <v>1200</v>
+      </c>
+      <c r="D30" s="19">
+        <v>50.83</v>
+      </c>
+      <c r="E30" s="20">
+        <v>76.459999999999994</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="21">
+        <f t="shared" si="0"/>
+        <v>0.33520795187025892</v>
+      </c>
+      <c r="H30" s="19">
+        <v>14.82</v>
+      </c>
+      <c r="I30" s="19">
+        <v>10.46</v>
+      </c>
+      <c r="J30" s="19">
+        <v>1.53</v>
+      </c>
+      <c r="K30" s="19">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L30" s="19">
+        <v>7.5825799999999999E-2</v>
+      </c>
+      <c r="M30" s="19">
+        <v>7.4814199999999997E-2</v>
+      </c>
+      <c r="N30" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="13">
+        <v>6</v>
+      </c>
+      <c r="C37" s="14">
+        <v>400</v>
+      </c>
+      <c r="D37" s="23">
+        <f t="shared" ref="D37:E41" si="1">AVERAGE(D6,D11,D16,D21,D26)</f>
+        <v>40.81</v>
+      </c>
+      <c r="E37" s="23">
+        <f t="shared" si="1"/>
+        <v>51.890000000000008</v>
+      </c>
+      <c r="F37" s="23"/>
+      <c r="G37" s="5">
+        <f>-(D37-E37)/E37</f>
+        <v>0.21352861823087307</v>
+      </c>
+      <c r="H37" s="23">
+        <f t="shared" ref="H37:N41" si="2">AVERAGE(H6,H11,H16,H21,H26)</f>
+        <v>17.893999999999998</v>
+      </c>
+      <c r="I37" s="23">
+        <f t="shared" si="2"/>
+        <v>15.321999999999999</v>
+      </c>
+      <c r="J37" s="26">
+        <f t="shared" si="2"/>
+        <v>2.0260000000000002</v>
+      </c>
+      <c r="K37" s="26">
+        <f t="shared" si="2"/>
+        <v>1.528</v>
+      </c>
+      <c r="L37" s="24">
+        <f t="shared" si="2"/>
+        <v>8.2686000000000009E-2</v>
+      </c>
+      <c r="M37" s="24">
+        <f t="shared" si="2"/>
+        <v>7.6065520000000011E-2</v>
+      </c>
+      <c r="N37" s="25">
+        <f t="shared" si="2"/>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="13">
+        <v>1</v>
+      </c>
+      <c r="C38" s="14">
+        <v>600</v>
+      </c>
+      <c r="D38" s="23">
+        <f t="shared" si="1"/>
+        <v>41.855999999999995</v>
+      </c>
+      <c r="E38" s="23">
+        <f t="shared" si="1"/>
+        <v>57.515999999999998</v>
+      </c>
+      <c r="F38" s="23"/>
+      <c r="G38" s="5">
+        <f>-(D38-E38)/E38</f>
+        <v>0.27227206342582938</v>
+      </c>
+      <c r="H38" s="23">
+        <f t="shared" si="2"/>
+        <v>17.594000000000001</v>
+      </c>
+      <c r="I38" s="23">
+        <f t="shared" si="2"/>
+        <v>12.796000000000001</v>
+      </c>
+      <c r="J38" s="26">
+        <f t="shared" si="2"/>
+        <v>1.9219999999999999</v>
+      </c>
+      <c r="K38" s="26">
+        <f t="shared" si="2"/>
+        <v>1.45</v>
+      </c>
+      <c r="L38" s="24">
+        <f t="shared" si="2"/>
+        <v>7.9668226000000009E-2</v>
+      </c>
+      <c r="M38" s="24">
+        <f t="shared" si="2"/>
+        <v>7.9125319999999999E-2</v>
+      </c>
+      <c r="N38" s="25">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="13">
+        <v>4</v>
+      </c>
+      <c r="C39" s="14">
+        <v>800</v>
+      </c>
+      <c r="D39" s="23">
+        <f t="shared" si="1"/>
+        <v>43.263999999999996</v>
+      </c>
+      <c r="E39" s="23">
+        <f t="shared" si="1"/>
+        <v>63.3</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="5">
+        <f>-(D39-E39)/E39</f>
+        <v>0.31652448657187998</v>
+      </c>
+      <c r="H39" s="23">
+        <f t="shared" si="2"/>
+        <v>17.07</v>
+      </c>
+      <c r="I39" s="23">
+        <f t="shared" si="2"/>
+        <v>11.978</v>
+      </c>
+      <c r="J39" s="26">
+        <f t="shared" si="2"/>
+        <v>1.798</v>
+      </c>
+      <c r="K39" s="26">
+        <f t="shared" si="2"/>
+        <v>1.3479999999999996</v>
+      </c>
+      <c r="L39" s="24">
+        <f t="shared" si="2"/>
+        <v>7.7063640000000003E-2</v>
+      </c>
+      <c r="M39" s="24">
+        <f t="shared" si="2"/>
+        <v>7.8862600000000005E-2</v>
+      </c>
+      <c r="N39" s="25">
+        <f t="shared" si="2"/>
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="13">
+        <v>7</v>
+      </c>
+      <c r="C40" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D40" s="23">
+        <f t="shared" si="1"/>
+        <v>46.585999999999999</v>
+      </c>
+      <c r="E40" s="23">
+        <f t="shared" si="1"/>
+        <v>68.823999999999998</v>
+      </c>
+      <c r="F40" s="23"/>
+      <c r="G40" s="5">
+        <f>-(D40-E40)/E40</f>
+        <v>0.32311402998953853</v>
+      </c>
+      <c r="H40" s="23">
+        <f t="shared" si="2"/>
+        <v>15.981999999999999</v>
+      </c>
+      <c r="I40" s="23">
+        <f t="shared" si="2"/>
+        <v>11.398</v>
+      </c>
+      <c r="J40" s="26">
+        <f t="shared" si="2"/>
+        <v>1.6180000000000003</v>
+      </c>
+      <c r="K40" s="26">
+        <f t="shared" si="2"/>
+        <v>1.29</v>
+      </c>
+      <c r="L40" s="24">
+        <f t="shared" si="2"/>
+        <v>7.4433655999999987E-2</v>
+      </c>
+      <c r="M40" s="24">
+        <f t="shared" si="2"/>
+        <v>7.8807199999999994E-2</v>
+      </c>
+      <c r="N40" s="25">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="13">
+        <v>8</v>
+      </c>
+      <c r="C41" s="14">
+        <v>1200</v>
+      </c>
+      <c r="D41" s="23">
+        <f t="shared" si="1"/>
+        <v>48.532000000000004</v>
+      </c>
+      <c r="E41" s="23">
+        <f t="shared" si="1"/>
+        <v>72.149999999999991</v>
+      </c>
+      <c r="F41" s="23"/>
+      <c r="G41" s="5">
+        <f>-(D41-E41)/E41</f>
+        <v>0.3273458073458072</v>
+      </c>
+      <c r="H41" s="23">
+        <f t="shared" si="2"/>
+        <v>15.388</v>
+      </c>
+      <c r="I41" s="23">
+        <f t="shared" si="2"/>
+        <v>11.2</v>
+      </c>
+      <c r="J41" s="26">
+        <f t="shared" si="2"/>
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="K41" s="26">
+        <f t="shared" si="2"/>
+        <v>1.2440000000000002</v>
+      </c>
+      <c r="L41" s="24">
+        <f t="shared" si="2"/>
+        <v>7.4837860000000006E-2</v>
+      </c>
+      <c r="M41" s="24">
+        <f t="shared" si="2"/>
+        <v>7.6676599999999998E-2</v>
+      </c>
+      <c r="N41" s="25">
+        <f t="shared" si="2"/>
+        <v>35.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3108,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979C2EAF-FEED-4955-BE2F-492EEFD618AC}">
   <dimension ref="A3:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixing the bug for separating path with more than one rear-end conflict zones + adding new paths
</commit_message>
<xml_diff>
--- a/IEEETransactionOnIntelligent/scenarios (version 1).xlsb.xlsx
+++ b/IEEETransactionOnIntelligent/scenarios (version 1).xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\matlab_workspace\SchedulingSimulation\IEEETransactionOnIntelligent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20A8D33-7522-4D98-839B-A5BA00A1E414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98358BD8-D8C4-445C-A378-54AF1CE3C753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43425" yWindow="3645" windowWidth="15300" windowHeight="7815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40770" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TrafficMetric" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
   <si>
     <t>u_min</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Seed42</t>
+  </si>
+  <si>
+    <t>The seed number is for the random generator in Matlab</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -618,6 +621,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1661,7 +1667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB574D0-D7A2-47DE-BC32-9F6E57DEC63E}">
   <dimension ref="A3:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -3106,7 +3112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9648945-6AF8-4AFE-93CD-85E1ADD724BE}">
   <dimension ref="A3:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -4561,10 +4567,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979C2EAF-FEED-4955-BE2F-492EEFD618AC}">
-  <dimension ref="A3:S49"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:M14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4589,6 +4595,21 @@
     <col min="20" max="16384" width="8.88671875" style="30"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+    </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -6100,11 +6121,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>